<commit_message>
Change column 'Part Description' to 'Description' [BOM]
The updated database mappings overwrites the component description. To
get those descriptions in the BOM the spreadsheet template should refer
to 'Description'.
</commit_message>
<xml_diff>
--- a/circuit_board/altium_bom_template_dig_v2020.xlsx
+++ b/circuit_board/altium_bom_template_dig_v2020.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augusto.fraga\repos\rtm-lamp-hw\circuit_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_4CB97A76634040A03323F9A2429B374FFC148C48" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CCF3E3-DB95-45DC-989B-C4D96352FB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8208" yWindow="-14400" windowWidth="24000" windowHeight="13212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -71,9 +71,6 @@
     <t>Column=Part Number</t>
   </si>
   <si>
-    <t>Column=Part Description</t>
-  </si>
-  <si>
     <t>Column=Value</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   <si>
     <t>Column=Quantity</t>
   </si>
+  <si>
+    <t>Column=Description</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,6 +171,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -301,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,6 +357,7 @@
     <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
@@ -1494,10 +1502,10 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:I4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -1519,7 +1527,7 @@
     <col min="18" max="18" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="12.75" customHeight="1">
+    <row r="1" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1541,7 +1549,7 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="57" customHeight="1">
+    <row r="2" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1561,7 +1569,7 @@
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
     </row>
-    <row r="3" spans="1:18" ht="24.6">
+    <row r="3" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1583,7 +1591,7 @@
       <c r="Q3" s="17"/>
       <c r="R3" s="17"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
@@ -1619,8 +1627,8 @@
       </c>
       <c r="R4" s="19"/>
     </row>
-    <row r="5" spans="1:18" ht="7.5" customHeight="1"/>
-    <row r="6" spans="1:18" s="1" customFormat="1" ht="39" customHeight="1">
+    <row r="5" spans="1:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:18" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1631,56 +1639,56 @@
         <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="Q6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="R6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1696,7 +1704,7 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1716,7 +1724,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1736,7 +1744,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1756,7 +1764,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1776,7 +1784,7 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1796,7 +1804,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1816,7 +1824,7 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1836,7 +1844,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1856,7 +1864,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1876,7 +1884,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1896,7 +1904,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1916,7 +1924,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1936,7 +1944,7 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1956,7 +1964,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1976,7 +1984,7 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1996,7 +2004,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2016,7 +2024,7 @@
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2036,7 +2044,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2056,7 +2064,7 @@
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2076,7 +2084,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2096,7 +2104,7 @@
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2116,7 +2124,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2136,7 +2144,7 @@
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2156,7 +2164,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2176,7 +2184,7 @@
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2196,7 +2204,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2216,7 +2224,7 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2236,7 +2244,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2256,7 +2264,7 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2276,7 +2284,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2296,7 +2304,7 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2316,7 +2324,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2336,7 +2344,7 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2356,7 +2364,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2376,7 +2384,7 @@
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2396,7 +2404,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2416,7 +2424,7 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2436,7 +2444,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2456,7 +2464,7 @@
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2476,7 +2484,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2496,7 +2504,7 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2516,7 +2524,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2536,7 +2544,7 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2556,7 +2564,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2576,7 +2584,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2596,7 +2604,7 @@
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2616,7 +2624,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2636,7 +2644,7 @@
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2656,7 +2664,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2676,7 +2684,7 @@
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2696,7 +2704,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2716,7 +2724,7 @@
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2736,7 +2744,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change field name from 'Fitted' to 'Mounted' [bom]
The column label should be 'Column=Mounted' to match.
</commit_message>
<xml_diff>
--- a/circuit_board/altium_bom_template_dig_v2020.xlsx
+++ b/circuit_board/altium_bom_template_dig_v2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augusto.fraga\repos\rtm-lamp-hw\circuit_board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augusto.fraga\repos\lnls\rtm-lamp-hw\circuit_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CCF3E3-DB95-45DC-989B-C4D96352FB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1105DAEA-97D3-4A1E-9B84-72F59C0D9631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>21/02/2020</t>
   </si>
   <si>
-    <t>Column=Fitted</t>
-  </si>
-  <si>
     <t>Column=Designator</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Column=Description</t>
+  </si>
+  <si>
+    <t>Column=Mounted</t>
   </si>
 </sst>
 </file>
@@ -330,6 +330,7 @@
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,7 +358,6 @@
     <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
@@ -1501,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1550,65 +1550,65 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="14"/>
       <c r="J4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1622,73 +1622,73 @@
       <c r="P4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="19"/>
+      <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:18" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="Q6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="R6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="8" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="20"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>

</xml_diff>